<commit_message>
combined plot - modified
</commit_message>
<xml_diff>
--- a/results/random_queries-2.xlsx
+++ b/results/random_queries-2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="45" windowWidth="11475" windowHeight="6465"/>
+    <workbookView xWindow="0" yWindow="105" windowWidth="11475" windowHeight="6405"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -597,11 +597,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -931,6 +927,16 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
         <c:crossAx val="99103744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
@@ -946,6 +952,16 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
         <c:crossAx val="553753600"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
@@ -976,7 +992,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr rtl="0">
-              <a:defRPr sz="1200"/>
+              <a:defRPr sz="1400"/>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
           </a:p>

</xml_diff>